<commit_message>
feat (robot): add report workflow
</commit_message>
<xml_diff>
--- a/Doc/Upload - Copy.xlsx
+++ b/Doc/Upload - Copy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eger\thesis\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F41ED6F-4F75-4405-9BCF-E5306758C7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0A37F7-3142-4628-8B82-94074061F1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Monitor</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Power Supplie</t>
   </si>
   <si>
-    <t>Computer Case</t>
-  </si>
-  <si>
     <t>Graphics Card</t>
   </si>
   <si>
@@ -92,7 +89,28 @@
     <t xml:space="preserve">Hard drive </t>
   </si>
   <si>
-    <t>AMD Ryzen 5 7600X</t>
+    <t>16 GB DDR5</t>
+  </si>
+  <si>
+    <t>Intel Core i5-13400F</t>
+  </si>
+  <si>
+    <t>Gaming Headset</t>
+  </si>
+  <si>
+    <t>Headset</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>500GB Kingston SSD</t>
+  </si>
+  <si>
+    <t>B650 AORUS</t>
+  </si>
+  <si>
+    <t>27" LG 27GR95QE</t>
   </si>
 </sst>
 </file>
@@ -137,9 +155,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -421,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD582D5D-D30B-46FF-8483-5D8A882FAC83}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,18 +462,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -464,10 +523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FF62CF-2793-4A0D-9ED0-43745A45E840}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,12 +546,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -512,22 +571,27 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -540,7 +604,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,26 +625,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(server): add SendEmail class to the server
</commit_message>
<xml_diff>
--- a/Doc/Upload - Copy.xlsx
+++ b/Doc/Upload - Copy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eger\thesis\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0A37F7-3142-4628-8B82-94074061F1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E30E1A7-5E25-4B88-BCD3-6CD196692561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Monitor</t>
   </si>
@@ -89,28 +89,10 @@
     <t xml:space="preserve">Hard drive </t>
   </si>
   <si>
-    <t>16 GB DDR5</t>
-  </si>
-  <si>
-    <t>Intel Core i5-13400F</t>
-  </si>
-  <si>
-    <t>Gaming Headset</t>
-  </si>
-  <si>
     <t>Headset</t>
   </si>
   <si>
     <t>Case</t>
-  </si>
-  <si>
-    <t>500GB Kingston SSD</t>
-  </si>
-  <si>
-    <t>B650 AORUS</t>
-  </si>
-  <si>
-    <t>27" LG 27GR95QE</t>
   </si>
 </sst>
 </file>
@@ -155,10 +137,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -440,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD582D5D-D30B-46FF-8483-5D8A882FAC83}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,54 +447,6 @@
       </c>
       <c r="B2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -571,7 +504,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -591,7 +524,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -604,7 +537,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,12 +591,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -909,20 +844,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5CB19FC-1968-49E0-884F-26F72BDB4530}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58105C1F-30FD-4489-9895-76158CD574CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
+    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -948,12 +884,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58105C1F-30FD-4489-9895-76158CD574CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5CB19FC-1968-49E0-884F-26F72BDB4530}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
-    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refact(server): modify ComputerParts and SerachResults modells
</commit_message>
<xml_diff>
--- a/Doc/Upload - Copy.xlsx
+++ b/Doc/Upload - Copy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eger\thesis\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E30E1A7-5E25-4B88-BCD3-6CD196692561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47697968-A092-4B02-973C-A748864D0F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Monitor</t>
   </si>
@@ -68,18 +68,6 @@
     <t>GeForce RTX 4060</t>
   </si>
   <si>
-    <t>Emag</t>
-  </si>
-  <si>
-    <t>http://emag.hu</t>
-  </si>
-  <si>
-    <t>Alza</t>
-  </si>
-  <si>
-    <t>http://alza.hu</t>
-  </si>
-  <si>
     <t>Pcx</t>
   </si>
   <si>
@@ -93,6 +81,12 @@
   </si>
   <si>
     <t>Case</t>
+  </si>
+  <si>
+    <t>Intel Core i5-13400F</t>
+  </si>
+  <si>
+    <t>B650 AORUS</t>
   </si>
 </sst>
 </file>
@@ -421,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD582D5D-D30B-46FF-8483-5D8A882FAC83}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,6 +441,22 @@
       </c>
       <c r="B2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -479,7 +489,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
@@ -504,7 +514,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -524,7 +534,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -534,10 +544,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,41 +574,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{DC05E364-51B2-40C0-AACC-ACBCA3D93755}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{9481404B-28C8-44BE-A270-A6F878179DFD}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{BBB29A76-B2A2-4FA6-822A-36E035B4664A}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{BBB29A76-B2A2-4FA6-822A-36E035B4664A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -844,21 +834,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58105C1F-30FD-4489-9895-76158CD574CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5CB19FC-1968-49E0-884F-26F72BDB4530}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
-    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -884,9 +873,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5CB19FC-1968-49E0-884F-26F72BDB4530}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58105C1F-30FD-4489-9895-76158CD574CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
+    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>